<commit_message>
save 05 09 2025
</commit_message>
<xml_diff>
--- a/4 четверть_14_JavaScript_crypto, JWT.xlsx
+++ b/4 четверть_14_JavaScript_crypto, JWT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexServHW\Desktop\GB_Developer_Workbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122FE785-3934-4F01-9202-CC85D30212FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C2D0FB-929D-46DA-815C-8DF444241AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5865" yWindow="-20100" windowWidth="23010" windowHeight="17460" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-13875" yWindow="-21720" windowWidth="51840" windowHeight="21120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Архитектура работы с паролем" sheetId="22" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="541">
   <si>
     <t>1</t>
   </si>
@@ -1449,9 +1449,6 @@
     <t>Signature:</t>
   </si>
   <si>
-    <t>Подпись, созданная путем шифрования Header и Payload с использованием секретного ключа (или пары ключей). Подпись гарантирует, что токен не был изменен после создания.</t>
-  </si>
-  <si>
     <t>Payload:</t>
   </si>
   <si>
@@ -1459,9 +1456,6 @@
   </si>
   <si>
     <t>Полезная нагрузка. Это сами данные (утверждения — "claims") о пользователе (например, userId: 123, username: "john", role: "admin").</t>
-  </si>
-  <si>
-    <t>Содержит информацию об алгоритме и типе токена.</t>
   </si>
   <si>
     <t>Служебная информация</t>
@@ -6139,73 +6133,6 @@
     <t>Архитектурно</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Критически важно для понимания!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Должен быть создан JWT со встроенной </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(1) цифровой подписью</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, а также данными в </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(2) зашифрованном</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> виде</t>
-    </r>
-  </si>
-  <si>
     <t>Sign</t>
   </si>
   <si>
@@ -7010,99 +6937,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Для правильной реализации jwt необходимо сохранять </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>secret</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>в переменных среды приложения</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, чтобы он не был виден в файлах исполнения программы.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">JWT = цифровая подпись для 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>любой</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> передаваемой информации между клиентом сервером 
-Важно! </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>сам информация должна быть отдельно зашифрована</t>
     </r>
   </si>
   <si>
@@ -8709,17 +8543,352 @@
     <t>JSON Web Token - Современный подход
 Возможность сделать jwt методы асинхронными</t>
   </si>
+  <si>
+    <t>Содержит метаданные о токене, например, алгоритм подписи (например, HS256, RS256) и тип токена.
+Пример: {"alg": "HS256", "typ": "JWT"}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Это то, что создается с помощью secretOrPrivateKey. Подпись вычисляется путем </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>хэширования</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> объединенных и закодированных header и payload с использованием</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (1) секретного ключа</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> и </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(2)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>алгоритма, указанного в заголовке.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Для правильной реализации jwt необходимо сохранять </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>secret</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>в переменных среды приложения</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, чтобы он не был виден в файлах исполнения программы.
+1 Secret нужен для </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>доступа</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> к </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>хэшированной с секретным ключем</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (см Crypto - хэширование с секретом) подписи.
+2 Secret может быть в виде </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.pem, const key = crypto.randomBytes(32);</t>
+    </r>
+  </si>
+  <si>
+    <t>JWT не хэшируется и не шифруется</t>
+  </si>
+  <si>
+    <t>JWT не хэшируется и не шифруется, он просто кодирован в Base64</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Критически важно для понимания!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+JWT создается со встроенной 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(1 - данные в сообщение хэшируются с секретным ключем = цифровая подпись) цифровой подписью</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, 
+а также данными в </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(2 - данные необходимо шифровать отдельно, тк jwt не делает этого, если необходимо) зашифрованном</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> виде</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">JWT = цифровая подпись для 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>любой</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> передаваемой информации между клиентом сервером 
+Важно! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>сама информация должна быть отдельно зашифрована</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="34" x14ac:knownFonts="1">
+  <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -9074,9 +9243,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -9087,13 +9256,13 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -9106,88 +9275,88 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -9196,13 +9365,13 @@
     <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -9211,40 +9380,46 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -9271,14 +9446,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>132566</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>77731</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1201159</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>1541318</xdr:rowOff>
+      <xdr:colOff>1197349</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>1545128</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9897,79 +10072,79 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C3" s="23" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="72" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C11" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C12" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C14" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
@@ -9993,32 +10168,32 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C16" s="23" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C17" s="52" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="18" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B18" s="42" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C18" s="42" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="52" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D19" s="2"/>
       <c r="F19" s="1"/>
@@ -10040,10 +10215,10 @@
     <row r="20" spans="1:22" s="7" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C20" s="37" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D20" s="2"/>
       <c r="F20" s="1"/>
@@ -10064,11 +10239,11 @@
     </row>
     <row r="21" spans="1:22" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D21" s="2"/>
       <c r="F21" s="1"/>
@@ -10089,11 +10264,11 @@
     </row>
     <row r="22" spans="1:22" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D22" s="4"/>
       <c r="F22" s="1"/>
@@ -10114,99 +10289,99 @@
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B23" s="10" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C24" s="42" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B25" s="42" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C25" s="42" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>207</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>210</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="29" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C31" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="32" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C32" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C33" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C34" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C35" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="36" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B36" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -10224,7 +10399,7 @@
   <dimension ref="A1:V30"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10280,28 +10455,28 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C2" s="26" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="53" t="s">
+        <v>158</v>
+      </c>
+      <c r="C3" s="30" t="s">
         <v>128</v>
-      </c>
-      <c r="B3" s="53" t="s">
-        <v>160</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>130</v>
       </c>
       <c r="D3" s="30"/>
       <c r="E3" s="30"/>
     </row>
     <row r="4" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" s="30" t="s">
         <v>129</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
@@ -10326,157 +10501,157 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C7" s="26" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B12" s="35" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D12" s="36" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E12" s="37"/>
     </row>
     <row r="13" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="39" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C13" s="30"/>
       <c r="D13" s="34" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="187.2" x14ac:dyDescent="0.3">
       <c r="C14" s="30"/>
-      <c r="D14" s="30" t="s">
-        <v>195</v>
+      <c r="D14" s="58" t="s">
+        <v>193</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="40" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B15" s="33" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E15" s="33" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" spans="1:22" ht="244.8" x14ac:dyDescent="0.3">
       <c r="B17" s="30" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="41" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B18" s="33" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D18" s="33" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E18" s="38"/>
     </row>
     <row r="19" spans="1:22" ht="144" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E19" s="30" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E20" s="2"/>
     </row>
@@ -10502,62 +10677,62 @@
     </row>
     <row r="23" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C23" s="34" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="25" spans="1:22" ht="244.8" x14ac:dyDescent="0.3">
       <c r="C25" s="30" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="26" spans="1:22" ht="316.8" x14ac:dyDescent="0.3">
       <c r="C26" s="30" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B27" s="35" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C27" s="36" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:22" ht="158.4" x14ac:dyDescent="0.3">
       <c r="B28" s="30" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D28" s="30"/>
       <c r="E28" s="30"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B29" s="35" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C29" s="36" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:22" ht="216" x14ac:dyDescent="0.3">
       <c r="B30" s="30" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D30" s="30"/>
       <c r="E30" s="30"/>
@@ -10576,8 +10751,8 @@
   </sheetPr>
   <dimension ref="A1:V74"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10632,26 +10807,26 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C2" s="26" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="30" t="s">
         <v>128</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="53" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" s="30" t="s">
         <v>129</v>
-      </c>
-      <c r="B4" s="53" t="s">
-        <v>161</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>131</v>
       </c>
       <c r="D4" s="30"/>
     </row>
@@ -10678,13 +10853,13 @@
       <c r="A7" s="12"/>
       <c r="B7" s="13"/>
       <c r="C7" s="26" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D7" s="13"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
@@ -10692,41 +10867,41 @@
     </row>
     <row r="9" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B9" s="13"/>
       <c r="C9" s="13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D9" s="13"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B10" s="13"/>
       <c r="C10" s="16" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D10" s="13"/>
     </row>
     <row r="11" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B11" s="13"/>
       <c r="C11" s="13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D11" s="13"/>
     </row>
     <row r="12" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B12" s="13"/>
       <c r="C12" s="16" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D12" s="13"/>
     </row>
@@ -10734,16 +10909,16 @@
       <c r="A13" s="12"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D13" s="13"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
@@ -10752,16 +10927,16 @@
       <c r="A15" s="13"/>
       <c r="B15" s="13"/>
       <c r="C15" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D15" s="13"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="24" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
@@ -11091,7 +11266,7 @@
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="26" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D30" s="13"/>
       <c r="E30" s="7"/>
@@ -11118,7 +11293,7 @@
         <v>21</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
@@ -11236,7 +11411,7 @@
         <v>32</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C35" s="13"/>
       <c r="D35" s="13"/>
@@ -11571,7 +11746,7 @@
       <c r="A52" s="13"/>
       <c r="B52" s="13"/>
       <c r="C52" s="13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D52" s="13"/>
     </row>
@@ -11740,7 +11915,7 @@
       <c r="A60" s="13"/>
       <c r="B60" s="13"/>
       <c r="C60" s="26" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D60" s="13"/>
       <c r="F60" s="1"/>
@@ -11784,13 +11959,13 @@
       <c r="U61" s="2"/>
       <c r="V61" s="1"/>
     </row>
-    <row r="62" spans="1:22" s="7" customFormat="1" ht="345.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:22" s="7" customFormat="1" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A62" s="13"/>
       <c r="B62" s="13" t="s">
         <v>73</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D62" s="13"/>
       <c r="F62" s="1"/>
@@ -12075,8 +12250,8 @@
   </sheetPr>
   <dimension ref="A1:V68"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12131,105 +12306,105 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C2" s="23" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="37" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="55" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="42"/>
       <c r="B5" s="42" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="55" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="42"/>
       <c r="C7" s="42" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="55" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="42"/>
       <c r="C9" s="4" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="42"/>
       <c r="C10" s="4" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="42"/>
       <c r="C11" s="4" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="42"/>
       <c r="C12" s="4" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="42"/>
       <c r="C13" s="4" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="55" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="42"/>
       <c r="B15" s="45"/>
       <c r="C15" s="45" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="44"/>
       <c r="B16" s="45"/>
       <c r="C16" s="45" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="44"/>
       <c r="B17" s="45"/>
       <c r="C17" s="45" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="18" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="44"/>
       <c r="B18" s="45"/>
       <c r="C18" s="45" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.3">
@@ -12253,33 +12428,33 @@
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C22" s="23" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="23" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C23" s="52" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="24" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A24" s="44"/>
       <c r="B24" s="46" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C24" s="37" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="25" spans="1:22" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="44" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B25" s="45"/>
       <c r="C25" s="45" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D25" s="2"/>
       <c r="F25" s="1"/>
@@ -12300,11 +12475,11 @@
     </row>
     <row r="26" spans="1:22" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="45" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B26" s="49"/>
       <c r="C26" s="46" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D26" s="2"/>
       <c r="F26" s="1"/>
@@ -12325,7 +12500,7 @@
     </row>
     <row r="27" spans="1:22" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B27" s="45"/>
       <c r="C27" s="45"/>
@@ -12350,7 +12525,7 @@
       <c r="A28" s="44"/>
       <c r="B28" s="45"/>
       <c r="C28" s="45" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D28" s="4"/>
       <c r="F28" s="1"/>
@@ -12373,26 +12548,26 @@
       <c r="A29" s="44"/>
       <c r="B29" s="45"/>
       <c r="C29" s="46" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="30" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="44"/>
       <c r="B30" s="45"/>
       <c r="C30" s="36" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="31" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="44"/>
       <c r="B31" s="45"/>
       <c r="C31" s="37" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="32" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="50" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B32" s="45"/>
       <c r="C32" s="47"/>
@@ -12401,32 +12576,32 @@
       <c r="A33" s="44"/>
       <c r="B33" s="45"/>
       <c r="C33" s="46" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A34" s="44"/>
       <c r="B34" s="45"/>
       <c r="C34" s="46" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="35" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="44"/>
       <c r="B35" s="43" t="s">
+        <v>293</v>
+      </c>
+      <c r="C35" s="46" t="s">
         <v>295</v>
-      </c>
-      <c r="C35" s="46" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="36" spans="1:22" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="44"/>
       <c r="B36" s="43" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C36" s="46" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="1"/>
@@ -12449,7 +12624,7 @@
     </row>
     <row r="37" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="51" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B37" s="45"/>
       <c r="C37" s="47"/>
@@ -12474,11 +12649,11 @@
     </row>
     <row r="38" spans="1:22" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A38" s="46" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B38" s="45"/>
       <c r="C38" s="46" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E38" s="7"/>
       <c r="F38" s="1"/>
@@ -12503,7 +12678,7 @@
       <c r="A39" s="44"/>
       <c r="B39" s="45"/>
       <c r="C39" s="46" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E39" s="7"/>
       <c r="F39" s="1"/>
@@ -12528,7 +12703,7 @@
       <c r="A40" s="44"/>
       <c r="B40" s="45"/>
       <c r="C40" s="46" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="1"/>
@@ -12553,7 +12728,7 @@
       <c r="A41" s="44"/>
       <c r="B41" s="45"/>
       <c r="C41" s="46" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E41" s="7"/>
       <c r="F41" s="1"/>
@@ -12576,7 +12751,7 @@
     </row>
     <row r="42" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B42" s="45"/>
       <c r="C42" s="47"/>
@@ -12601,7 +12776,7 @@
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A43" s="44" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B43" s="45"/>
       <c r="C43" s="47"/>
@@ -12609,70 +12784,70 @@
     <row r="44" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A44" s="44"/>
       <c r="B44" s="46" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="45" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C45" s="42" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="46" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C46" s="42" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="47" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C47" s="42" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B48" s="4" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C49" s="42" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B50" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C51" s="42" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B53" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C54" s="4" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B55" s="42" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="C56" s="4" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
@@ -12735,10 +12910,10 @@
     <tabColor rgb="FF7030A0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V133"/>
+  <dimension ref="A1:V135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12793,205 +12968,160 @@
     </row>
     <row r="2" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C2" s="23" t="s">
-        <v>439</v>
+        <v>540</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="54" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
       <c r="C4" s="37" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="52" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C6" s="42" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-      <c r="U7" s="5"/>
-    </row>
-    <row r="8" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C8" s="23" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A5" s="54" t="s">
+        <v>537</v>
+      </c>
+      <c r="C5" s="59"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="C6" s="59" t="s">
         <v>538</v>
       </c>
     </row>
+    <row r="7" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="52" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="C8" s="58" t="s">
+        <v>536</v>
+      </c>
+    </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" ht="259.2" x14ac:dyDescent="0.3">
-      <c r="C10" s="42" t="s">
+      <c r="A9" s="3"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="U9" s="5"/>
+    </row>
+    <row r="10" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C10" s="23" t="s">
         <v>533</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="C12" s="42" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>524</v>
+      </c>
+      <c r="C13" s="50" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="B15" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="C15" s="42" t="s">
         <v>529</v>
       </c>
-      <c r="C11" s="50" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B12" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="C12" s="1" t="s">
+    </row>
+    <row r="16" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="50" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="B13" s="2" t="s">
+    <row r="17" spans="1:22" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="C17" s="42" t="s">
         <v>532</v>
       </c>
-      <c r="C13" s="42" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="50" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="C15" s="42" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="5"/>
-      <c r="U18" s="5"/>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="C19" s="23" t="s">
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A20" s="3"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="5"/>
+      <c r="U20" s="5"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C21" s="23" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B21" s="17" t="s">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="C21" s="17" t="s">
+    </row>
+    <row r="23" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B23" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="15" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="15" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="13"/>
-      <c r="B23" s="16" t="s">
+    <row r="25" spans="1:22" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="13"/>
+      <c r="B25" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C25" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="D23" s="13"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="P23" s="2"/>
-      <c r="Q23" s="2"/>
-      <c r="R23" s="2"/>
-      <c r="S23" s="1"/>
-      <c r="T23" s="8"/>
-      <c r="U23" s="2"/>
-      <c r="V23" s="1"/>
-    </row>
-    <row r="24" spans="1:22" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="D24" s="13"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="P24" s="2"/>
-      <c r="Q24" s="2"/>
-      <c r="R24" s="2"/>
-      <c r="S24" s="1"/>
-      <c r="T24" s="8"/>
-      <c r="U24" s="2"/>
-      <c r="V24" s="1"/>
-    </row>
-    <row r="25" spans="1:22" s="7" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>112</v>
-      </c>
+      <c r="D25" s="13"/>
       <c r="F25" s="1"/>
       <c r="G25" s="2"/>
       <c r="H25" s="1"/>
@@ -13008,13 +13138,17 @@
       <c r="U25" s="2"/>
       <c r="V25" s="1"/>
     </row>
-    <row r="26" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
+    <row r="26" spans="1:22" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" s="13"/>
       <c r="F26" s="1"/>
       <c r="G26" s="2"/>
       <c r="H26" s="1"/>
@@ -13031,17 +13165,19 @@
       <c r="U26" s="2"/>
       <c r="V26" s="1"/>
     </row>
-    <row r="27" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D27" s="4"/>
+    <row r="27" spans="1:22" s="7" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="F27" s="1"/>
       <c r="G27" s="2"/>
       <c r="H27" s="1"/>
@@ -13058,832 +13194,872 @@
       <c r="U27" s="2"/>
       <c r="V27" s="1"/>
     </row>
-    <row r="28" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="8"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="1"/>
+    </row>
+    <row r="29" spans="1:22" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B28" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="C28" s="17" t="s">
+      <c r="B29" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="29" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+      <c r="C29" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="D29" s="4"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="8"/>
+      <c r="U29" s="2"/>
+      <c r="V29" s="1"/>
+    </row>
+    <row r="30" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C30" s="58" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="10" t="s">
+      <c r="B31" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" s="58" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B32" s="17"/>
+    </row>
+    <row r="33" spans="1:21" ht="60" x14ac:dyDescent="0.3">
+      <c r="A33" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33" s="29" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" ht="30" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B30" s="17"/>
-    </row>
-    <row r="31" spans="1:22" ht="60" x14ac:dyDescent="0.3">
-      <c r="A31" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" s="27" t="s">
+      <c r="C34" s="28" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" ht="45" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C31" s="29" t="s">
+      <c r="C35" s="28" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="32" spans="1:22" ht="30" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C32" s="28" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" ht="45" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C33" s="28" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A35" s="3"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-      <c r="M35" s="3"/>
-      <c r="N35" s="3"/>
-      <c r="P35" s="5"/>
-      <c r="Q35" s="5"/>
-      <c r="R35" s="5"/>
-      <c r="S35" s="5"/>
-      <c r="U35" s="5"/>
-    </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="C36" s="23" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A37" s="9" t="s">
-        <v>385</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>455</v>
-      </c>
-      <c r="C37" s="1"/>
-      <c r="D37" s="42" t="s">
-        <v>411</v>
-      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A37" s="3"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="P37" s="5"/>
+      <c r="Q37" s="5"/>
+      <c r="R37" s="5"/>
+      <c r="S37" s="5"/>
+      <c r="U37" s="5"/>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A38" s="24" t="s">
-        <v>440</v>
-      </c>
-      <c r="C38" s="1"/>
-      <c r="D38" s="42"/>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D39" s="42"/>
-    </row>
-    <row r="40" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="B40" s="42" t="s">
-        <v>418</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>416</v>
-      </c>
+      <c r="C38" s="23" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="42" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A40" s="24" t="s">
+        <v>435</v>
+      </c>
+      <c r="C40" s="1"/>
       <c r="D40" s="42"/>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="D41" s="42"/>
+    </row>
+    <row r="42" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D41" s="42"/>
-    </row>
-    <row r="42" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="B42" s="56" t="s">
-        <v>449</v>
-      </c>
-      <c r="C42" s="42" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="B42" s="42" t="s">
+        <v>415</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="D42" s="42"/>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="B43" s="42" t="s">
-        <v>478</v>
-      </c>
-      <c r="C43" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="D43" s="42"/>
+    </row>
+    <row r="44" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="D43" s="42" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" ht="144" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
-        <v>448</v>
-      </c>
       <c r="B44" s="56" t="s">
-        <v>526</v>
-      </c>
-      <c r="C44" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="C44" s="42" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="B45" s="42" t="s">
+        <v>473</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="D45" s="42" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" ht="144" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
         <v>443</v>
       </c>
-      <c r="D44" s="42" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="B45" s="42" t="s">
-        <v>478</v>
-      </c>
-      <c r="C45" s="42" t="s">
-        <v>442</v>
-      </c>
-      <c r="D45" s="42" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="B46" s="42" t="s">
-        <v>478</v>
-      </c>
-      <c r="C46" s="42" t="s">
-        <v>444</v>
+      <c r="B46" s="56" t="s">
+        <v>521</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>438</v>
       </c>
       <c r="D46" s="42" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="47" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="B47" s="42" t="s">
-        <v>478</v>
-      </c>
-      <c r="D47" s="42"/>
+        <v>473</v>
+      </c>
+      <c r="C47" s="42" t="s">
+        <v>437</v>
+      </c>
+      <c r="D47" s="42" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="48" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="B48" s="42" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="C48" s="42" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="D48" s="42" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>423</v>
+        <v>418</v>
+      </c>
+      <c r="B49" s="42" t="s">
+        <v>473</v>
       </c>
       <c r="D49" s="42"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="D50" s="42"/>
+        <v>419</v>
+      </c>
+      <c r="B50" s="42" t="s">
+        <v>473</v>
+      </c>
+      <c r="C50" s="42" t="s">
+        <v>440</v>
+      </c>
+      <c r="D50" s="42" t="s">
+        <v>434</v>
+      </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="D51" s="42"/>
     </row>
-    <row r="52" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A52" s="2" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="D52" s="42"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="D53" s="42"/>
+    </row>
+    <row r="54" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="C54" s="42" t="s">
+        <v>427</v>
+      </c>
+      <c r="D54" s="42"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="C55" s="42" t="s">
+        <v>428</v>
+      </c>
+      <c r="D55" s="42"/>
+    </row>
+    <row r="56" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="C52" s="42" t="s">
-        <v>430</v>
-      </c>
-      <c r="D52" s="42"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="C53" s="42" t="s">
-        <v>431</v>
-      </c>
-      <c r="D53" s="42"/>
-    </row>
-    <row r="54" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
+      <c r="C56" s="42" t="s">
         <v>429</v>
       </c>
-      <c r="C54" s="42" t="s">
-        <v>432</v>
-      </c>
-      <c r="D54" s="42"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="10" t="s">
-        <v>491</v>
-      </c>
-      <c r="C55" s="42"/>
-      <c r="D55" s="42"/>
-    </row>
-    <row r="56" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A56" s="33" t="s">
-        <v>386</v>
-      </c>
-      <c r="C56" s="1"/>
-    </row>
-    <row r="57" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A57" s="2"/>
-      <c r="B57" s="42" t="s">
-        <v>398</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D56" s="42"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="10" t="s">
+        <v>486</v>
+      </c>
+      <c r="C57" s="42"/>
+      <c r="D57" s="42"/>
+    </row>
+    <row r="58" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" s="33" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="C58" s="1"/>
     </row>
-    <row r="59" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
       <c r="B59" s="42" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="33" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="C60" s="1"/>
     </row>
     <row r="61" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
       <c r="B61" s="42" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="33" t="s">
+        <v>387</v>
+      </c>
+      <c r="C62" s="1"/>
+    </row>
+    <row r="63" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A63" s="2"/>
+      <c r="B63" s="42" t="s">
+        <v>389</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="33" t="s">
+        <v>396</v>
+      </c>
+      <c r="C64" s="1"/>
+    </row>
+    <row r="65" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B65" s="11" t="s">
+        <v>398</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A66" s="9" t="s">
         <v>399</v>
       </c>
-      <c r="C62" s="1"/>
-    </row>
-    <row r="63" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B63" s="11" t="s">
+      <c r="C66" s="1"/>
+    </row>
+    <row r="67" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A67" s="2"/>
+      <c r="C67" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="D67" s="2"/>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A68" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="C63" s="2" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="9" t="s">
-        <v>402</v>
-      </c>
-      <c r="C64" s="1"/>
-    </row>
-    <row r="65" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A65" s="2"/>
-      <c r="C65" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="D65" s="2"/>
-    </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A66" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="C66" s="2" t="s">
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A69" s="53" t="s">
         <v>404</v>
       </c>
-      <c r="D66" s="2"/>
-    </row>
-    <row r="67" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A67" s="53" t="s">
-        <v>407</v>
-      </c>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
-    </row>
-    <row r="68" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A68" s="2"/>
-      <c r="B68" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="D68" s="2"/>
-    </row>
-    <row r="69" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A69" s="2"/>
-      <c r="B69" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>409</v>
-      </c>
+      <c r="C69" s="2"/>
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A70" s="2"/>
       <c r="B70" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A71" s="2"/>
+      <c r="B71" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="C70" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="D70" s="2"/>
-    </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A71" s="3"/>
-      <c r="B71" s="5"/>
-      <c r="C71" s="6"/>
-      <c r="D71" s="6"/>
-      <c r="F71" s="3"/>
-      <c r="G71" s="5"/>
-      <c r="H71" s="3"/>
-      <c r="I71" s="3"/>
-      <c r="K71" s="3"/>
-      <c r="L71" s="3"/>
-      <c r="M71" s="3"/>
-      <c r="N71" s="3"/>
-      <c r="P71" s="5"/>
-      <c r="Q71" s="5"/>
-      <c r="R71" s="5"/>
-      <c r="S71" s="5"/>
-      <c r="U71" s="5"/>
-    </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="C72" s="23" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="73" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A73" s="10" t="s">
-        <v>450</v>
-      </c>
-      <c r="B73" s="2" t="s">
+      <c r="D71" s="2"/>
+    </row>
+    <row r="72" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A72" s="2"/>
+      <c r="B72" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D72" s="2"/>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A73" s="3"/>
+      <c r="B73" s="5"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="5"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="3"/>
+      <c r="K73" s="3"/>
+      <c r="L73" s="3"/>
+      <c r="M73" s="3"/>
+      <c r="N73" s="3"/>
+      <c r="P73" s="5"/>
+      <c r="Q73" s="5"/>
+      <c r="R73" s="5"/>
+      <c r="S73" s="5"/>
+      <c r="U73" s="5"/>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="C74" s="23" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A75" s="10" t="s">
+        <v>445</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A76" s="2"/>
+      <c r="B76" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="C76" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2" t="s">
+      <c r="D76" s="2"/>
+    </row>
+    <row r="77" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A77" s="2"/>
+      <c r="B77" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="D77" s="2"/>
+    </row>
+    <row r="78" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A78" s="2" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="74" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A74" s="2"/>
-      <c r="B74" s="2" t="s">
+      <c r="C78" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="C74" s="2" t="s">
-        <v>459</v>
-      </c>
-      <c r="D74" s="2"/>
-    </row>
-    <row r="75" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A75" s="2"/>
-      <c r="B75" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="D75" s="2"/>
-    </row>
-    <row r="76" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="2" t="s">
-        <v>456</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="D76" s="2"/>
-    </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A77" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="C77" s="2"/>
-      <c r="D77" s="2"/>
-    </row>
-    <row r="78" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A78" s="2" t="s">
-        <v>460</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>461</v>
-      </c>
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>462</v>
-      </c>
-      <c r="B79" s="42" t="s">
-        <v>487</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>463</v>
-      </c>
+        <v>414</v>
+      </c>
+      <c r="C79" s="2"/>
       <c r="D79" s="2"/>
     </row>
     <row r="80" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>464</v>
+        <v>455</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
       <c r="D80" s="2"/>
     </row>
     <row r="81" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="B81" s="42" t="s">
+        <v>482</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="D81" s="2"/>
+    </row>
+    <row r="82" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A82" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="D82" s="2"/>
+    </row>
+    <row r="83" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A83" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="B83" s="42" t="s">
+        <v>474</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A84" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="B84" s="42" t="s">
+        <v>483</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="C85" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="B81" s="42" t="s">
-        <v>479</v>
-      </c>
-      <c r="C81" s="2" t="s">
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="C86" s="2"/>
+    </row>
+    <row r="87" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A87" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="B87" s="42" t="s">
+        <v>484</v>
+      </c>
+      <c r="C87" s="2" t="s">
         <v>468</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A82" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="B82" s="42" t="s">
-        <v>488</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" s="2" t="s">
-        <v>471</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="C84" s="2"/>
-    </row>
-    <row r="85" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A85" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="B85" s="42" t="s">
-        <v>489</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A86" s="2" t="s">
-        <v>474</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A87" s="2" t="s">
-        <v>476</v>
-      </c>
-      <c r="B87" s="11" t="s">
-        <v>490</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="D87" s="42" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="B88" s="42" t="s">
+        <v>469</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A89" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="B89" s="11" t="s">
         <v>485</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="C89" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="D89" s="42" t="s">
         <v>481</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A89" s="2" t="s">
-        <v>482</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
-        <v>484</v>
+        <v>475</v>
+      </c>
+      <c r="B90" s="42" t="s">
+        <v>480</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" s="10" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A91" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A92" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="10" t="s">
+        <v>489</v>
+      </c>
+      <c r="C93" s="2"/>
+      <c r="D93" s="2"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" s="33" t="s">
+        <v>448</v>
+      </c>
+      <c r="D94" s="2"/>
+    </row>
+    <row r="95" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A95" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="C95" s="42" t="s">
+        <v>492</v>
+      </c>
+      <c r="D95" s="2"/>
+    </row>
+    <row r="96" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A96" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="D96" s="2"/>
+    </row>
+    <row r="97" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A97" s="33" t="s">
+        <v>447</v>
+      </c>
+      <c r="C97" s="2"/>
+      <c r="D97" s="2"/>
+    </row>
+    <row r="98" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A98" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="D98" s="2"/>
+    </row>
+    <row r="99" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A99" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="C91" s="2"/>
-      <c r="D91" s="2"/>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A92" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="D92" s="2"/>
-    </row>
-    <row r="93" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A93" s="2" t="s">
-        <v>496</v>
-      </c>
-      <c r="C93" s="42" t="s">
+      <c r="C99" s="42" t="s">
         <v>497</v>
-      </c>
-      <c r="D93" s="2"/>
-    </row>
-    <row r="94" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A94" s="2" t="s">
-        <v>495</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>498</v>
-      </c>
-      <c r="D94" s="2"/>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95" s="33" t="s">
-        <v>452</v>
-      </c>
-      <c r="C95" s="2"/>
-      <c r="D95" s="2"/>
-    </row>
-    <row r="96" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A96" s="2" t="s">
-        <v>500</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="D96" s="2"/>
-    </row>
-    <row r="97" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A97" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="C97" s="42" t="s">
-        <v>502</v>
-      </c>
-      <c r="D97" s="2"/>
-    </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A98" s="10" t="s">
-        <v>494</v>
-      </c>
-      <c r="C98" s="2"/>
-      <c r="D98" s="2"/>
-    </row>
-    <row r="99" spans="1:21" ht="72" x14ac:dyDescent="0.3">
-      <c r="A99" s="2"/>
-      <c r="B99" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>504</v>
       </c>
       <c r="D99" s="2"/>
     </row>
     <row r="100" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A100" s="10" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
     </row>
-    <row r="101" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:21" ht="72" x14ac:dyDescent="0.3">
       <c r="A101" s="2"/>
       <c r="B101" s="2" t="s">
-        <v>507</v>
+        <v>498</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="D101" s="2"/>
     </row>
-    <row r="102" spans="1:21" ht="72" x14ac:dyDescent="0.3">
-      <c r="A102" s="2"/>
-      <c r="B102" s="2" t="s">
-        <v>505</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>508</v>
-      </c>
+    <row r="102" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A102" s="10" t="s">
+        <v>489</v>
+      </c>
+      <c r="C102" s="2"/>
       <c r="D102" s="2"/>
     </row>
-    <row r="103" spans="1:21" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A103" s="2"/>
+      <c r="B103" s="2" t="s">
+        <v>502</v>
+      </c>
       <c r="C103" s="2" t="s">
-        <v>511</v>
+        <v>501</v>
       </c>
       <c r="D103" s="2"/>
     </row>
-    <row r="104" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:21" ht="72" x14ac:dyDescent="0.3">
       <c r="A104" s="2"/>
+      <c r="B104" s="2" t="s">
+        <v>500</v>
+      </c>
       <c r="C104" s="2" t="s">
-        <v>510</v>
+        <v>503</v>
       </c>
       <c r="D104" s="2"/>
     </row>
-    <row r="105" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:21" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A105" s="2"/>
       <c r="C105" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="D105" s="2"/>
+    </row>
+    <row r="106" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A106" s="2"/>
+      <c r="C106" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="D106" s="2"/>
+    </row>
+    <row r="107" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A107" s="2"/>
+      <c r="C107" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="D107" s="2"/>
+    </row>
+    <row r="108" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A108" s="2"/>
+      <c r="C108" s="2"/>
+      <c r="D108" s="2"/>
+    </row>
+    <row r="109" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A109" s="3"/>
+      <c r="B109" s="5"/>
+      <c r="C109" s="6"/>
+      <c r="D109" s="6"/>
+      <c r="F109" s="3"/>
+      <c r="G109" s="5"/>
+      <c r="H109" s="3"/>
+      <c r="I109" s="3"/>
+      <c r="K109" s="3"/>
+      <c r="L109" s="3"/>
+      <c r="M109" s="3"/>
+      <c r="N109" s="3"/>
+      <c r="P109" s="5"/>
+      <c r="Q109" s="5"/>
+      <c r="R109" s="5"/>
+      <c r="S109" s="5"/>
+      <c r="U109" s="5"/>
+    </row>
+    <row r="110" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="C110" s="23" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="111" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A111" s="10" t="s">
+        <v>507</v>
+      </c>
+      <c r="C111" s="2"/>
+      <c r="D111" s="2"/>
+    </row>
+    <row r="112" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A112" s="57" t="s">
+        <v>508</v>
+      </c>
+      <c r="C112" s="1"/>
+      <c r="D112" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="D105" s="2"/>
-    </row>
-    <row r="106" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A106" s="2"/>
-      <c r="C106" s="2"/>
-      <c r="D106" s="2"/>
-    </row>
-    <row r="107" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A107" s="3"/>
-      <c r="B107" s="5"/>
-      <c r="C107" s="6"/>
-      <c r="D107" s="6"/>
-      <c r="F107" s="3"/>
-      <c r="G107" s="5"/>
-      <c r="H107" s="3"/>
-      <c r="I107" s="3"/>
-      <c r="K107" s="3"/>
-      <c r="L107" s="3"/>
-      <c r="M107" s="3"/>
-      <c r="N107" s="3"/>
-      <c r="P107" s="5"/>
-      <c r="Q107" s="5"/>
-      <c r="R107" s="5"/>
-      <c r="S107" s="5"/>
-      <c r="U107" s="5"/>
-    </row>
-    <row r="108" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="C108" s="23" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="109" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A109" s="10" t="s">
-        <v>512</v>
-      </c>
-      <c r="C109" s="2"/>
-      <c r="D109" s="2"/>
-    </row>
-    <row r="110" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A110" s="57" t="s">
-        <v>513</v>
-      </c>
-      <c r="C110" s="1"/>
-      <c r="D110" s="2" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="111" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A111" s="2"/>
-      <c r="C111" s="2" t="s">
-        <v>516</v>
-      </c>
-      <c r="D111" s="2"/>
-    </row>
-    <row r="112" spans="1:21" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A112" s="2"/>
-      <c r="C112" s="2" t="s">
-        <v>515</v>
-      </c>
-      <c r="D112" s="2"/>
-    </row>
-    <row r="113" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A113" s="57" t="s">
-        <v>518</v>
-      </c>
-      <c r="C113" s="2"/>
-      <c r="D113" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="114" spans="1:21" ht="144" x14ac:dyDescent="0.3">
+    </row>
+    <row r="113" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A113" s="2"/>
+      <c r="C113" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="D113" s="2"/>
+    </row>
+    <row r="114" spans="1:21" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A114" s="2"/>
       <c r="C114" s="2" t="s">
-        <v>520</v>
+        <v>510</v>
       </c>
       <c r="D114" s="2"/>
     </row>
-    <row r="115" spans="1:21" ht="144" x14ac:dyDescent="0.3">
-      <c r="A115" s="2"/>
-      <c r="C115" s="2" t="s">
-        <v>519</v>
-      </c>
-      <c r="D115" s="2"/>
-    </row>
-    <row r="116" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A116" s="57" t="s">
-        <v>523</v>
-      </c>
-      <c r="D116" s="2" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="117" spans="1:21" ht="72" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A115" s="57" t="s">
+        <v>513</v>
+      </c>
+      <c r="C115" s="2"/>
+      <c r="D115" s="2" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="116" spans="1:21" ht="144" x14ac:dyDescent="0.3">
+      <c r="A116" s="2"/>
+      <c r="C116" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="D116" s="2"/>
+    </row>
+    <row r="117" spans="1:21" ht="144" x14ac:dyDescent="0.3">
       <c r="A117" s="2"/>
       <c r="C117" s="2" t="s">
-        <v>524</v>
+        <v>514</v>
       </c>
       <c r="D117" s="2"/>
     </row>
-    <row r="118" spans="1:21" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A118" s="2"/>
-      <c r="C118" s="2" t="s">
-        <v>525</v>
-      </c>
-      <c r="D118" s="2"/>
-    </row>
-    <row r="119" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A118" s="57" t="s">
+        <v>518</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="119" spans="1:21" ht="72" x14ac:dyDescent="0.3">
       <c r="A119" s="2"/>
-      <c r="C119" s="2"/>
+      <c r="C119" s="2" t="s">
+        <v>519</v>
+      </c>
       <c r="D119" s="2"/>
     </row>
-    <row r="120" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:21" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A120" s="2"/>
-      <c r="C120" s="2"/>
+      <c r="C120" s="2" t="s">
+        <v>520</v>
+      </c>
       <c r="D120" s="2"/>
     </row>
     <row r="121" spans="1:21" x14ac:dyDescent="0.3">
@@ -13892,108 +14068,118 @@
       <c r="D121" s="2"/>
     </row>
     <row r="122" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A122" s="3"/>
-      <c r="B122" s="5"/>
-      <c r="C122" s="6"/>
-      <c r="D122" s="6"/>
-      <c r="F122" s="3"/>
-      <c r="G122" s="5"/>
-      <c r="H122" s="3"/>
-      <c r="I122" s="3"/>
-      <c r="K122" s="3"/>
-      <c r="L122" s="3"/>
-      <c r="M122" s="3"/>
-      <c r="N122" s="3"/>
-      <c r="P122" s="5"/>
-      <c r="Q122" s="5"/>
-      <c r="R122" s="5"/>
-      <c r="S122" s="5"/>
-      <c r="U122" s="5"/>
+      <c r="A122" s="2"/>
+      <c r="C122" s="2"/>
+      <c r="D122" s="2"/>
     </row>
     <row r="123" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="C123" s="23" t="s">
-        <v>382</v>
-      </c>
+      <c r="A123" s="2"/>
+      <c r="C123" s="2"/>
+      <c r="D123" s="2"/>
     </row>
     <row r="124" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A124" s="9" t="s">
+      <c r="A124" s="3"/>
+      <c r="B124" s="5"/>
+      <c r="C124" s="6"/>
+      <c r="D124" s="6"/>
+      <c r="F124" s="3"/>
+      <c r="G124" s="5"/>
+      <c r="H124" s="3"/>
+      <c r="I124" s="3"/>
+      <c r="K124" s="3"/>
+      <c r="L124" s="3"/>
+      <c r="M124" s="3"/>
+      <c r="N124" s="3"/>
+      <c r="P124" s="5"/>
+      <c r="Q124" s="5"/>
+      <c r="R124" s="5"/>
+      <c r="S124" s="5"/>
+      <c r="U124" s="5"/>
+    </row>
+    <row r="125" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="C125" s="23" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="126" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A126" s="9" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="127" spans="1:21" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="C127" s="42" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="128" spans="1:21" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A128" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B128" s="42" t="s">
+        <v>371</v>
+      </c>
+      <c r="C128" s="42" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="125" spans="1:21" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="C125" s="42" t="s">
+    <row r="129" spans="1:3" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A129" s="42" t="s">
+        <v>364</v>
+      </c>
+      <c r="B129" s="42" t="s">
+        <v>379</v>
+      </c>
+      <c r="C129" s="42" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A130" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="C130" s="42" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="126" spans="1:21" ht="230.4" x14ac:dyDescent="0.3">
-      <c r="A126" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="B126" s="42" t="s">
+    <row r="131" spans="1:3" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A131" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="C131" s="42" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A132" s="9" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A133" s="42" t="s">
+        <v>376</v>
+      </c>
+      <c r="C133" s="42" t="s">
         <v>373</v>
       </c>
-      <c r="C126" s="42" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="127" spans="1:21" ht="259.2" x14ac:dyDescent="0.3">
-      <c r="A127" s="42" t="s">
-        <v>366</v>
-      </c>
-      <c r="B127" s="42" t="s">
-        <v>381</v>
-      </c>
-      <c r="C127" s="42" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="128" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A128" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="C128" s="42" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A129" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="C129" s="42" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A130" s="9" t="s">
+    </row>
+    <row r="134" spans="1:3" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A134" s="42" t="s">
+        <v>375</v>
+      </c>
+      <c r="C134" s="42" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="331.2" x14ac:dyDescent="0.3">
+      <c r="A135" s="42" t="s">
+        <v>375</v>
+      </c>
+      <c r="C135" s="42" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A131" s="42" t="s">
-        <v>378</v>
-      </c>
-      <c r="C131" s="42" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" ht="374.4" x14ac:dyDescent="0.3">
-      <c r="A132" s="42" t="s">
-        <v>377</v>
-      </c>
-      <c r="C132" s="42" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" ht="331.2" x14ac:dyDescent="0.3">
-      <c r="A133" s="42" t="s">
-        <v>377</v>
-      </c>
-      <c r="C133" s="42" t="s">
-        <v>376</v>
-      </c>
-    </row>
   </sheetData>
-  <phoneticPr fontId="33" type="noConversion"/>
+  <phoneticPr fontId="35" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="10" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -14064,134 +14250,134 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C3" s="23" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" s="42"/>
       <c r="C4" s="42" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B5" s="42"/>
       <c r="C5" s="42"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="24" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B6" s="42"/>
       <c r="C6" s="42"/>
     </row>
     <row r="7" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B7" s="42" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" s="42"/>
       <c r="C8" s="42" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B9" s="42"/>
       <c r="C9" s="42" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B10" s="42" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="42"/>
       <c r="C11" s="42" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B12" s="42" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B13" s="42" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C13" s="42"/>
     </row>
     <row r="14" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="42"/>
       <c r="C14" s="42" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B15" s="42"/>
       <c r="C15" s="42" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B16" s="42"/>
       <c r="C16" s="42" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="17" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B17" s="42"/>
       <c r="C17" s="42" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="18" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B18" s="42"/>
       <c r="C18" s="42" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="19" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B19" s="42"/>
       <c r="C19" s="42" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="20" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B20" s="42" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C20" s="42" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B21" s="42"/>
       <c r="C21" s="42"/>
     </row>
     <row r="22" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B22" s="45"/>
       <c r="C22" s="45"/>
@@ -14214,7 +14400,7 @@
     </row>
     <row r="23" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="33" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B23" s="45"/>
       <c r="C23" s="46"/>
@@ -14238,7 +14424,7 @@
     <row r="24" spans="1:22" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="A24" s="45"/>
       <c r="B24" s="48" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C24" s="45"/>
       <c r="D24" s="2"/>
@@ -14261,10 +14447,10 @@
     <row r="25" spans="1:22" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="44"/>
       <c r="B25" s="48" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C25" s="46" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D25" s="4"/>
       <c r="F25" s="1"/>
@@ -14287,33 +14473,33 @@
       <c r="A26" s="44"/>
       <c r="B26" s="45"/>
       <c r="C26" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="27" spans="1:22" ht="72" x14ac:dyDescent="0.3">
       <c r="A27" s="44"/>
       <c r="B27" s="45"/>
       <c r="C27" s="46" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="44"/>
       <c r="B28" s="46"/>
       <c r="C28" s="46" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="29" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="44"/>
       <c r="B29" s="45"/>
       <c r="C29" s="46" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" s="24" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B30" s="45"/>
       <c r="C30" s="47"/>
@@ -14321,136 +14507,136 @@
     <row r="31" spans="1:22" ht="15" x14ac:dyDescent="0.3">
       <c r="A31" s="44"/>
       <c r="B31" s="48" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C31" s="47"/>
     </row>
     <row r="32" spans="1:22" ht="15" x14ac:dyDescent="0.3">
       <c r="A32" s="44"/>
       <c r="B32" s="48" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C32" s="46" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="44"/>
       <c r="B33" s="45"/>
       <c r="C33" s="46" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="44"/>
       <c r="B34" s="45"/>
       <c r="C34" s="46" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="44"/>
       <c r="B35" s="45"/>
       <c r="C35" s="46" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="44"/>
       <c r="B36" s="45"/>
       <c r="C36" s="46" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="24" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C39" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C40" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="24" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C42" s="42" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="24" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C44" s="42" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C46" s="42" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="24" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C49" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C50" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C51" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="C53" s="42" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>